<commit_message>
Latest update and edited testcases
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/loginData.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/loginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\selenium\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athira\git\repository\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152898FA-EA51-4424-AE82-397613AD25FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A86312-C160-40BB-855A-92F7FA4AF3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6ADC99FA-5585-4030-B756-15EA96C4463C}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -52,34 +52,26 @@
     <t>athiravj</t>
   </si>
   <si>
-    <t>TESTNG12</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>Abhiram</t>
-  </si>
-  <si>
-    <t>Abhiram@11</t>
+    <t>Marquetta</t>
+  </si>
+  <si>
+    <t>AngelCaridad</t>
+  </si>
+  <si>
+    <t>ang123Caridad</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,16 +94,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -482,50 +471,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1978C01-7CDB-4C0F-8D1F-0C9AE6EDD984}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" activeCellId="1" sqref="C1 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{D3F3632E-B74C-471A-B4EB-0B78D711F3E0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>